<commit_message>
"screen and component design"
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Necati\Desktop\NL\Kosmos Payroll\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\05_React_Native\Kosmos Payroll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72F49D7-B327-400E-A677-45ED4B84E6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0546A049-8D56-4909-AF3E-6D7B04F3125A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dashboard" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Employee Name</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>salary by month</t>
+  </si>
+  <si>
+    <t>Monthly Trends</t>
+  </si>
+  <si>
+    <t>Weekly Activity</t>
   </si>
 </sst>
 </file>
@@ -177,8 +183,8 @@
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>93776</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>273071</xdr:colOff>
       <xdr:row>72</xdr:row>
       <xdr:rowOff>27712</xdr:rowOff>
     </xdr:to>
@@ -221,8 +227,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>236718</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>416012</xdr:colOff>
       <xdr:row>109</xdr:row>
       <xdr:rowOff>84905</xdr:rowOff>
     </xdr:to>
@@ -397,8 +403,8 @@
       <xdr:rowOff>41413</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>262085</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>441379</xdr:colOff>
       <xdr:row>192</xdr:row>
       <xdr:rowOff>97627</xdr:rowOff>
     </xdr:to>
@@ -442,7 +448,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>45043</xdr:colOff>
+      <xdr:colOff>45042</xdr:colOff>
       <xdr:row>190</xdr:row>
       <xdr:rowOff>175918</xdr:rowOff>
     </xdr:to>
@@ -486,7 +492,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>374251</xdr:colOff>
+      <xdr:colOff>374252</xdr:colOff>
       <xdr:row>188</xdr:row>
       <xdr:rowOff>70316</xdr:rowOff>
     </xdr:to>
@@ -661,8 +667,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>351899</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>531193</xdr:colOff>
       <xdr:row>278</xdr:row>
       <xdr:rowOff>37167</xdr:rowOff>
     </xdr:to>
@@ -706,7 +712,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>280486</xdr:colOff>
+      <xdr:colOff>280487</xdr:colOff>
       <xdr:row>278</xdr:row>
       <xdr:rowOff>94315</xdr:rowOff>
     </xdr:to>
@@ -750,7 +756,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>404289</xdr:colOff>
+      <xdr:colOff>404288</xdr:colOff>
       <xdr:row>278</xdr:row>
       <xdr:rowOff>151470</xdr:rowOff>
     </xdr:to>
@@ -1278,8 +1284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1290,19 +1296,20 @@
     <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="16:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="15:18" x14ac:dyDescent="0.25">
       <c r="P3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="16:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="15:18" x14ac:dyDescent="0.25">
       <c r="P4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="16:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="15:18" x14ac:dyDescent="0.25">
       <c r="P5" t="s">
         <v>11</v>
       </c>
@@ -1310,9 +1317,17 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="16:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="15:18" x14ac:dyDescent="0.25">
+      <c r="O14" t="s">
+        <v>14</v>
+      </c>
       <c r="P14" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="15:18" x14ac:dyDescent="0.25">
+      <c r="O15" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="3:9" x14ac:dyDescent="0.25">

</xml_diff>